<commit_message>
basic models for most special pages
</commit_message>
<xml_diff>
--- a/backend/fares/sample.xlsx
+++ b/backend/fares/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzobule\Documents\flysolomons\website\backend\fares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52D33390-E825-435A-8F85-1593CAD58F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D0F83B-97D8-472C-B7E7-A3246062CA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48C9D2E8-62A9-4192-A748-43B4AC47E190}"/>
   </bookViews>
@@ -31,37 +31,37 @@
     <t>Currency</t>
   </si>
   <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Saver</t>
+  </si>
+  <si>
+    <t>SBD</t>
+  </si>
+  <si>
+    <t>HIR</t>
+  </si>
+  <si>
+    <t>BNE</t>
+  </si>
+  <si>
+    <t>Smart</t>
+  </si>
+  <si>
+    <t>Flexi</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
     <t>Trip Type</t>
   </si>
   <si>
-    <t>Origin</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>Saver</t>
-  </si>
-  <si>
-    <t>SBD</t>
-  </si>
-  <si>
-    <t>one way</t>
-  </si>
-  <si>
-    <t>HIR</t>
-  </si>
-  <si>
-    <t>BNE</t>
-  </si>
-  <si>
-    <t>Smart</t>
-  </si>
-  <si>
-    <t>Flexi</t>
-  </si>
-  <si>
-    <t>Business</t>
+    <t>One Way</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A60226B-8F4A-463B-ADFA-097CC7A29E3E}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -939,93 +941,93 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1990.99</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1590.99</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1890.99</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>5090.99</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
route page connected with backend, route section connected with backend as well
</commit_message>
<xml_diff>
--- a/backend/fares/sample.xlsx
+++ b/backend/fares/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzobule\Documents\flysolomons\website\backend\fares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D0F83B-97D8-472C-B7E7-A3246062CA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C372221E-5A7C-4E21-9A2D-468442EC4DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48C9D2E8-62A9-4192-A748-43B4AC47E190}"/>
   </bookViews>
@@ -46,22 +46,22 @@
     <t>HIR</t>
   </si>
   <si>
+    <t>Smart</t>
+  </si>
+  <si>
+    <t>Flexi</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Trip Type</t>
+  </si>
+  <si>
+    <t>One Way</t>
+  </si>
+  <si>
     <t>BNE</t>
-  </si>
-  <si>
-    <t>Smart</t>
-  </si>
-  <si>
-    <t>Flexi</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>Trip Type</t>
-  </si>
-  <si>
-    <t>One Way</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -961,18 +961,18 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>1590.99</v>
@@ -981,18 +981,18 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>1890.99</v>
@@ -1001,18 +1001,18 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>5090.99</v>
@@ -1021,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few adjustments for progress update
</commit_message>
<xml_diff>
--- a/backend/fares/sample.xlsx
+++ b/backend/fares/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzobule\Documents\flysolomons\website\backend\fares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00204137-FBA4-49CB-87DE-C624BD876936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498234CA-E8B1-4C24-B047-C9D387BF0D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48C9D2E8-62A9-4192-A748-43B4AC47E190}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48C9D2E8-62A9-4192-A748-43B4AC47E190}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>SBD</t>
   </si>
   <si>
-    <t>HIR</t>
-  </si>
-  <si>
     <t>Smart</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>One Way</t>
+  </si>
+  <si>
+    <t>BNE</t>
   </si>
   <si>
     <t>AKL</t>
@@ -925,7 +925,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,7 +941,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -961,10 +961,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -972,7 +972,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1590.99</v>
@@ -981,10 +981,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>1890.99</v>
@@ -1001,10 +1001,10 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>5090.99</v>
@@ -1021,10 +1021,10 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>

</xml_diff>